<commit_message>
trying to match the heat map to the initialized image
</commit_message>
<xml_diff>
--- a/monte_carlo/results/scenario1/heat_map.xlsx
+++ b/monte_carlo/results/scenario1/heat_map.xlsx
@@ -357,12 +357,15 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>10.5238995904687</v>
       </c>
@@ -379,7 +382,7 @@
         <v>8.3025034919180403</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2.3971909843905901</v>
       </c>
@@ -396,7 +399,7 @@
         <v>6.2734920586723302</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>-0.262118510999999</v>
       </c>
@@ -413,7 +416,7 @@
         <v>5.6319117762046202</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>-0.72899999999999998</v>
       </c>
@@ -430,7 +433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
trial 2 to make the heat same size with init pic
</commit_message>
<xml_diff>
--- a/monte_carlo/results/scenario1/heat_map.xlsx
+++ b/monte_carlo/results/scenario1/heat_map.xlsx
@@ -357,7 +357,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,7 +365,7 @@
     <col min="1" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>10.5238995904687</v>
       </c>
@@ -382,7 +382,7 @@
         <v>8.3025034919180403</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2.3971909843905901</v>
       </c>
@@ -399,7 +399,7 @@
         <v>6.2734920586723302</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>-0.262118510999999</v>
       </c>
@@ -416,7 +416,7 @@
         <v>5.6319117762046202</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>-0.72899999999999998</v>
       </c>
@@ -433,7 +433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>

</xml_diff>